<commit_message>
recurso solar y nubosidad actualizado
</commit_message>
<xml_diff>
--- a/data/Recurso_solar.xlsx
+++ b/data/Recurso_solar.xlsx
@@ -439,7 +439,7 @@
     <col width="6" customWidth="1" min="1" max="1"/>
     <col width="21" customWidth="1" min="2" max="2"/>
     <col width="10" customWidth="1" min="3" max="3"/>
-    <col width="8" customWidth="1" min="4" max="4"/>
+    <col width="9" customWidth="1" min="4" max="4"/>
     <col width="19" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
@@ -619,10 +619,10 @@
         <v>22.72</v>
       </c>
       <c r="D10" t="n">
-        <v>29.56</v>
+        <v>45.42</v>
       </c>
       <c r="E10" t="n">
-        <v>30.12</v>
+        <v>99.91</v>
       </c>
     </row>
     <row r="11">
@@ -638,10 +638,10 @@
         <v>285.24</v>
       </c>
       <c r="D11" t="n">
-        <v>371.15</v>
+        <v>464.39</v>
       </c>
       <c r="E11" t="n">
-        <v>30.12</v>
+        <v>62.81</v>
       </c>
     </row>
     <row r="12">
@@ -657,10 +657,10 @@
         <v>467.02</v>
       </c>
       <c r="D12" t="n">
-        <v>607.67</v>
+        <v>698.86</v>
       </c>
       <c r="E12" t="n">
-        <v>30.12</v>
+        <v>49.64</v>
       </c>
     </row>
     <row r="13">
@@ -676,10 +676,10 @@
         <v>604.9400000000001</v>
       </c>
       <c r="D13" t="n">
-        <v>787.13</v>
+        <v>871.8</v>
       </c>
       <c r="E13" t="n">
-        <v>30.12</v>
+        <v>44.11</v>
       </c>
     </row>
     <row r="14">
@@ -695,10 +695,10 @@
         <v>685</v>
       </c>
       <c r="D14" t="n">
-        <v>891.3</v>
+        <v>976.38</v>
       </c>
       <c r="E14" t="n">
-        <v>30.12</v>
+        <v>42.54</v>
       </c>
     </row>
     <row r="15">
@@ -714,10 +714,10 @@
         <v>700.6</v>
       </c>
       <c r="D15" t="n">
-        <v>911.6</v>
+        <v>1009.65</v>
       </c>
       <c r="E15" t="n">
-        <v>30.12</v>
+        <v>44.11</v>
       </c>
     </row>
     <row r="16">
@@ -733,10 +733,10 @@
         <v>650.34</v>
       </c>
       <c r="D16" t="n">
-        <v>846.21</v>
+        <v>973.1900000000001</v>
       </c>
       <c r="E16" t="n">
-        <v>30.12</v>
+        <v>49.64</v>
       </c>
     </row>
     <row r="17">
@@ -752,10 +752,10 @@
         <v>537.1</v>
       </c>
       <c r="D17" t="n">
-        <v>698.86</v>
+        <v>874.4299999999999</v>
       </c>
       <c r="E17" t="n">
-        <v>30.12</v>
+        <v>62.81</v>
       </c>
     </row>
     <row r="18">
@@ -771,10 +771,10 @@
         <v>372.54</v>
       </c>
       <c r="D18" t="n">
-        <v>484.74</v>
+        <v>744.75</v>
       </c>
       <c r="E18" t="n">
-        <v>30.12</v>
+        <v>99.91</v>
       </c>
     </row>
     <row r="19">
@@ -790,10 +790,10 @@
         <v>174.42</v>
       </c>
       <c r="D19" t="n">
-        <v>226.95</v>
+        <v>523.26</v>
       </c>
       <c r="E19" t="n">
-        <v>30.12</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20">
@@ -809,10 +809,10 @@
         <v>0.22</v>
       </c>
       <c r="D20" t="n">
-        <v>0.29</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>30.12</v>
+        <v>-100</v>
       </c>
     </row>
     <row r="21">
@@ -922,7 +922,7 @@
     <col width="6" customWidth="1" min="1" max="1"/>
     <col width="21" customWidth="1" min="2" max="2"/>
     <col width="10" customWidth="1" min="3" max="3"/>
-    <col width="9" customWidth="1" min="4" max="4"/>
+    <col width="8" customWidth="1" min="4" max="4"/>
     <col width="19" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
@@ -1068,10 +1068,10 @@
         <v>3.94</v>
       </c>
       <c r="D8" t="n">
-        <v>3.7</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>-6.22</v>
+        <v>-100</v>
       </c>
     </row>
     <row r="9">
@@ -1087,10 +1087,10 @@
         <v>213.04</v>
       </c>
       <c r="D9" t="n">
-        <v>199.8</v>
+        <v>85.61</v>
       </c>
       <c r="E9" t="n">
-        <v>-6.22</v>
+        <v>-59.81</v>
       </c>
     </row>
     <row r="10">
@@ -1106,10 +1106,10 @@
         <v>460.82</v>
       </c>
       <c r="D10" t="n">
-        <v>432.18</v>
+        <v>292.6</v>
       </c>
       <c r="E10" t="n">
-        <v>-6.22</v>
+        <v>-36.5</v>
       </c>
     </row>
     <row r="11">
@@ -1125,10 +1125,10 @@
         <v>509.32</v>
       </c>
       <c r="D11" t="n">
-        <v>477.66</v>
+        <v>374.14</v>
       </c>
       <c r="E11" t="n">
-        <v>-6.22</v>
+        <v>-26.54</v>
       </c>
     </row>
     <row r="12">
@@ -1144,10 +1144,10 @@
         <v>758.26</v>
       </c>
       <c r="D12" t="n">
-        <v>711.13</v>
+        <v>594.79</v>
       </c>
       <c r="E12" t="n">
-        <v>-6.22</v>
+        <v>-21.56</v>
       </c>
     </row>
     <row r="13">
@@ -1163,10 +1163,10 @@
         <v>971.72</v>
       </c>
       <c r="D13" t="n">
-        <v>911.3200000000001</v>
+        <v>785.83</v>
       </c>
       <c r="E13" t="n">
-        <v>-6.22</v>
+        <v>-19.13</v>
       </c>
     </row>
     <row r="14">
@@ -1182,10 +1182,10 @@
         <v>1125.48</v>
       </c>
       <c r="D14" t="n">
-        <v>1055.52</v>
+        <v>918.45</v>
       </c>
       <c r="E14" t="n">
-        <v>-6.22</v>
+        <v>-18.39</v>
       </c>
     </row>
     <row r="15">
@@ -1201,10 +1201,10 @@
         <v>1136.72</v>
       </c>
       <c r="D15" t="n">
-        <v>1066.07</v>
+        <v>919.27</v>
       </c>
       <c r="E15" t="n">
-        <v>-6.22</v>
+        <v>-19.13</v>
       </c>
     </row>
     <row r="16">
@@ -1220,10 +1220,10 @@
         <v>1076.84</v>
       </c>
       <c r="D16" t="n">
-        <v>1009.91</v>
+        <v>844.7</v>
       </c>
       <c r="E16" t="n">
-        <v>-6.22</v>
+        <v>-21.56</v>
       </c>
     </row>
     <row r="17">
@@ -1239,10 +1239,10 @@
         <v>950.52</v>
       </c>
       <c r="D17" t="n">
-        <v>891.4400000000001</v>
+        <v>698.24</v>
       </c>
       <c r="E17" t="n">
-        <v>-6.22</v>
+        <v>-26.54</v>
       </c>
     </row>
     <row r="18">
@@ -1258,10 +1258,10 @@
         <v>767.38</v>
       </c>
       <c r="D18" t="n">
-        <v>719.6799999999999</v>
+        <v>487.26</v>
       </c>
       <c r="E18" t="n">
-        <v>-6.22</v>
+        <v>-36.5</v>
       </c>
     </row>
     <row r="19">
@@ -1277,10 +1277,10 @@
         <v>542.38</v>
       </c>
       <c r="D19" t="n">
-        <v>508.67</v>
+        <v>217.96</v>
       </c>
       <c r="E19" t="n">
-        <v>-6.22</v>
+        <v>-59.81</v>
       </c>
     </row>
     <row r="20">
@@ -1296,10 +1296,10 @@
         <v>296.1</v>
       </c>
       <c r="D20" t="n">
-        <v>277.7</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>-6.22</v>
+        <v>-100</v>
       </c>
     </row>
     <row r="21">
@@ -1315,10 +1315,10 @@
         <v>61.52</v>
       </c>
       <c r="D21" t="n">
-        <v>57.7</v>
+        <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>-6.22</v>
+        <v>-100</v>
       </c>
     </row>
     <row r="22">
@@ -1503,13 +1503,13 @@
         <v>13</v>
       </c>
       <c r="F2" t="n">
-        <v>911.6</v>
+        <v>1009.65</v>
       </c>
       <c r="G2" t="n">
-        <v>243.98</v>
+        <v>299.26</v>
       </c>
       <c r="H2" t="n">
-        <v>5.855</v>
+        <v>7.182</v>
       </c>
       <c r="I2" t="n">
         <v>13</v>
@@ -1518,10 +1518,10 @@
         <v>11</v>
       </c>
       <c r="K2" t="n">
-        <v>30.12</v>
+        <v>59.6</v>
       </c>
       <c r="L2" t="n">
-        <v>1.355</v>
+        <v>2.682</v>
       </c>
     </row>
     <row r="3">
@@ -1543,13 +1543,13 @@
         <v>13</v>
       </c>
       <c r="F3" t="n">
-        <v>1066.07</v>
+        <v>919.27</v>
       </c>
       <c r="G3" t="n">
-        <v>346.77</v>
+        <v>259.12</v>
       </c>
       <c r="H3" t="n">
-        <v>8.321999999999999</v>
+        <v>6.219</v>
       </c>
       <c r="I3" t="n">
         <v>13</v>
@@ -1558,10 +1558,10 @@
         <v>14</v>
       </c>
       <c r="K3" t="n">
-        <v>-6.22</v>
+        <v>-29.92</v>
       </c>
       <c r="L3" t="n">
-        <v>-0.552</v>
+        <v>-2.655</v>
       </c>
     </row>
   </sheetData>
@@ -1631,7 +1631,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>20°</t>
+          <t>35°</t>
         </is>
       </c>
     </row>
@@ -1679,7 +1679,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2025-07-04 11:00:10</t>
+          <t>2025-07-10 12:37:53</t>
         </is>
       </c>
     </row>

</xml_diff>